<commit_message>
Otimização .degree com numba
</commit_message>
<xml_diff>
--- a/dbdp_instances/incgraph_25_25_0.065_0.2_1.xlsx
+++ b/dbdp_instances/incgraph_25_25_0.065_0.2_1.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno Ferrari\Documents\Bruno\2019\2s\MC\artigos revisão\Artigos Mes\GD\bdp\dbdp_instances\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3670BF05-552A-482B-A766-D4C560949D8B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC01E870-0200-41E5-860B-0B0644144406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{75E468A2-3D70-49CF-A2E2-2A35575198B7}"/>
+    <workbookView xWindow="5760" yWindow="1455" windowWidth="19620" windowHeight="8610" activeTab="1" xr2:uid="{75E468A2-3D70-49CF-A2E2-2A35575198B7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="x" sheetId="1" r:id="rId1"/>
+    <sheet name="y" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -130,16 +130,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>56</xdr:col>
-      <xdr:colOff>90122</xdr:colOff>
+      <xdr:col>73</xdr:col>
+      <xdr:colOff>207353</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>98181</xdr:rowOff>
+      <xdr:rowOff>83528</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>73</xdr:col>
-      <xdr:colOff>232473</xdr:colOff>
+      <xdr:col>91</xdr:col>
+      <xdr:colOff>107916</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>40657</xdr:rowOff>
+      <xdr:rowOff>26004</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -162,7 +162,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13630276" y="860181"/>
+          <a:off x="17857911" y="845528"/>
           <a:ext cx="4252755" cy="2990476"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -475,7 +475,7 @@
   <dimension ref="A1:AL32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AL4" sqref="AL4"/>
+      <selection activeCell="Z36" sqref="Z36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3876,8 +3876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1738F21B-825D-40A3-984E-D1E5F94CD8AE}">
   <dimension ref="A1:AL32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AU22" sqref="AU22"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AP30" sqref="AP30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>